<commit_message>
working on new Layout with voltage to frequency AD654 "U2"
</commit_message>
<xml_diff>
--- a/CURRENT/openSX70_ALPHA_V6-2-3-20181104.xlsx
+++ b/CURRENT/openSX70_ALPHA_V6-2-3-20181104.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>Qty</t>
   </si>
@@ -165,18 +165,9 @@
     <t>LD11172.5V</t>
   </si>
   <si>
-    <t>VBPW34S</t>
-  </si>
-  <si>
-    <t>SOD6439X130N</t>
-  </si>
-  <si>
     <t>D3</t>
   </si>
   <si>
-    <t>VBPW34SR Series 60 V 940 nm 50 mA 215 mW Surface Mount Silicon PIN Photodiode</t>
-  </si>
-  <si>
     <t>R2, R4</t>
   </si>
   <si>
@@ -213,9 +204,6 @@
     <t>LD1117-2.5</t>
   </si>
   <si>
-    <t>687106183722</t>
-  </si>
-  <si>
     <t>CONN FFC BTM 6POS 0.5MM SMD R/A</t>
   </si>
   <si>
@@ -235,13 +223,22 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>FPC 6-way</t>
+  </si>
+  <si>
+    <t>SFH2430</t>
+  </si>
+  <si>
+    <t>OSRAM SFH2430</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,8 +373,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,8 +562,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -688,126 +699,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -853,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -866,26 +757,11 @@
     <xf numFmtId="49" fontId="9" fillId="5" borderId="10" xfId="9" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="10" xfId="35" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="26" borderId="10" xfId="35" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="15" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="6" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="6" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="9" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="15" xfId="9" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="14" xfId="35" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="26" borderId="15" xfId="35" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="26" borderId="10" xfId="35" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="15" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="18" fillId="5" borderId="10" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1210,405 +1086,419 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="76.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="76.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5">
+        <v>301010089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="5">
+        <v>301010090</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="17">
-        <v>301010089</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="4">
+      <c r="G7" s="5">
+        <v>301010241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5">
+        <v>301010291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="17">
-        <v>301010090</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="G9" s="5">
+        <v>301010299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="7">
+        <v>302010138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="4">
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="7">
+        <v>302010103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="D13" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="4">
-        <v>2</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="17">
-        <v>301010241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2">
         <v>1</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="17">
-        <v>301010291</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="17">
-        <v>301010299</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="6">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="19">
-        <v>302010138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="19">
-        <v>302010103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="8">
-        <v>2</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="10">
-        <v>2</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="G16" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="G17" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="2">
+      <c r="C18" s="2">
         <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26" t="s">
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="27">
+      <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="D19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="29" t="s">
-        <v>69</v>
+      <c r="G19" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="2.3228346456692917" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F</oddHeader>
     <oddFooter>&amp;C&amp;D</oddFooter>

</xml_diff>